<commit_message>
comparing busburst siol moisture models
</commit_message>
<xml_diff>
--- a/Analyses/soilmoisture/mod_comparison.xlsx
+++ b/Analyses/soilmoisture/mod_comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>22 divergent transitions</t>
+  </si>
+  <si>
+    <t>test5cent.rstanarm</t>
+  </si>
+  <si>
+    <t>4 divergent transitions</t>
   </si>
 </sst>
 </file>
@@ -136,8 +142,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,7 +194,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -202,6 +214,9 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -221,6 +236,9 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,7 +568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -558,10 +576,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="9" width="18.33203125" customWidth="1"/>
+    <col min="2" max="8" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -586,8 +605,11 @@
       <c r="I1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -613,10 +635,13 @@
         <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -644,8 +669,11 @@
       <c r="I3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -667,11 +695,17 @@
       <c r="G4">
         <v>47</v>
       </c>
+      <c r="H4">
+        <v>47</v>
+      </c>
       <c r="I4">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -699,8 +733,11 @@
       <c r="I5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -725,8 +762,11 @@
       <c r="I6">
         <v>9514</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>9514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -745,11 +785,17 @@
       <c r="G7" s="2">
         <v>108.3216</v>
       </c>
+      <c r="H7">
+        <v>95.28</v>
+      </c>
       <c r="I7">
+        <v>96.169168999999997</v>
+      </c>
+      <c r="J7">
         <v>108.93</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -768,11 +814,17 @@
       <c r="G8" s="2">
         <v>-4.2267000000000001</v>
       </c>
+      <c r="H8">
+        <v>-9.69</v>
+      </c>
       <c r="I8">
+        <v>-9.3518709999999992</v>
+      </c>
+      <c r="J8">
         <v>-3.97</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -791,11 +843,17 @@
       <c r="G9" s="2">
         <v>-44.487299999999998</v>
       </c>
+      <c r="H9">
+        <v>-1.69</v>
+      </c>
       <c r="I9">
+        <v>-1.6437349999999999</v>
+      </c>
+      <c r="J9">
         <v>-50.35</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -814,58 +872,35 @@
       <c r="G10" s="2">
         <v>5.6989999999999998</v>
       </c>
+      <c r="H10">
+        <v>0.7</v>
+      </c>
       <c r="I10">
+        <v>0.72115099999999999</v>
+      </c>
+      <c r="J10">
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="5:8">
+    <row r="21" spans="5:5">
       <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="5:8">
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" t="s">
         <v>2</v>
-      </c>
-      <c r="F22">
-        <v>0.3</v>
-      </c>
-      <c r="G22">
-        <v>0.1</v>
-      </c>
-      <c r="H22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="23" spans="5:8">
-      <c r="F23">
-        <f>C7+(C8*F21)+(C9*F22) + (C10*F21*F22)</f>
-        <v>42.508447399999994</v>
-      </c>
-      <c r="G23">
-        <f>C7+(C8*G21)+(C9*G22) + (C10*G21*G22)</f>
-        <v>36.332109799999991</v>
-      </c>
-      <c r="H23">
-        <f>C7+(C8*H21)+(C9*H22) + (C10*H21*H22)</f>
-        <v>102.3586426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more bb soil moisture forecasts
</commit_message>
<xml_diff>
--- a/Analyses/soilmoisture/mod_comparison.xlsx
+++ b/Analyses/soilmoisture/mod_comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>4 divergent transitions</t>
+  </si>
+  <si>
+    <t>test5.rstanarm</t>
   </si>
 </sst>
 </file>
@@ -142,8 +145,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -194,7 +201,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -217,6 +224,8 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +248,8 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,19 +579,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="8" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="2" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -608,8 +620,11 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -625,23 +640,26 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -672,8 +690,11 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -704,8 +725,11 @@
       <c r="J4">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -736,8 +760,11 @@
       <c r="J5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -753,20 +780,20 @@
       <c r="E6">
         <v>12549</v>
       </c>
-      <c r="F6">
-        <v>9514</v>
-      </c>
       <c r="G6">
         <v>9514</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>9514</v>
       </c>
       <c r="J6">
         <v>9514</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>9514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -779,23 +806,24 @@
       <c r="E7" s="2">
         <v>109.811468</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
         <v>96.404399999999995</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>108.3216</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>95.28</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>96.169168999999997</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>108.93</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -808,23 +836,24 @@
       <c r="E8" s="2">
         <v>-3.4174959999999999</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
         <v>-9.3283000000000005</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-4.2267000000000001</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>-9.69</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>-9.3518709999999992</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>-3.97</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -837,23 +866,24 @@
       <c r="E9" s="2">
         <v>-42.018143999999999</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
         <v>-1.5954999999999999</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-44.487299999999998</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>-1.69</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>-1.6437349999999999</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-50.35</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -866,30 +896,30 @@
       <c r="E10">
         <v>1.116792</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0.78739999999999999</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>5.6989999999999998</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.7</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.72115099999999999</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="G11" t="s">
+    <row r="11" spans="1:11">
+      <c r="H11" t="s">
         <v>16</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>